<commit_message>
Add kitten vs sitting for verify
</commit_message>
<xml_diff>
--- a/cseditdistance/data/compare_ieditdistance.xlsx
+++ b/cseditdistance/data/compare_ieditdistance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1fastaccess\RPA\RPA_source\Information Retrieval\iEditDistance\cseditdistance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF60EB39-3BAB-4478-9528-16A535328825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDB320B-3FE8-4F30-9177-428A129A788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10095" tabRatio="481" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15495" tabRatio="442" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20230130" sheetId="1" r:id="rId1"/>
@@ -1521,7 +1521,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1563,13 +1563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1603,9 +1597,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -3753,10 +3744,10 @@
       <c r="D1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>191</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -3805,7 +3796,7 @@
       <c r="F3" s="9">
         <v>0.8</v>
       </c>
-      <c r="G3" s="30" t="str">
+      <c r="G3" s="5" t="str">
         <f>"result = r.Calculate(" &amp; """" &amp; Table2[[#This Row],[source1]] &amp; """" &amp; " , " &amp; """" &amp; Table2[[#This Row],[source2]] &amp; """" &amp; ");"</f>
         <v>result = r.Calculate("ABBYYY" , "ABBY");</v>
       </c>
@@ -4592,8 +4583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20B42DC-F998-4970-830E-0B33D7D593EC}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4611,7 +4602,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>263</v>
       </c>
       <c r="B2" t="s">
@@ -4642,14 +4633,14 @@
       <c r="A4" t="s">
         <v>266</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="29"/>
       <c r="F4" t="s">
         <v>256</v>
       </c>
@@ -4658,7 +4649,7 @@
       <c r="A5" t="s">
         <v>267</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>265</v>
       </c>
     </row>
@@ -4666,10 +4657,10 @@
       <c r="A6" t="s">
         <v>252</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="29" t="s">
         <v>265</v>
       </c>
     </row>
@@ -4712,7 +4703,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="29" t="s">
         <v>262</v>
       </c>
     </row>
@@ -4821,29 +4812,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613DAD67-06E2-429E-B285-9BB401CAD1C8}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+    <sheetView zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>258</v>
       </c>
     </row>
@@ -4858,7 +4849,7 @@
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>281</v>
       </c>
     </row>
@@ -4939,36 +4930,36 @@
       <c r="B9" s="14">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="17" t="s">
         <v>239</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="15" t="s">
         <v>241</v>
       </c>
       <c r="J9" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="17"/>
+      <c r="L9" s="26"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
@@ -4979,22 +4970,22 @@
       <c r="B10" s="14">
         <v>2</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>240</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="16" t="s">
         <v>243</v>
       </c>
       <c r="I10" s="15" t="s">
@@ -5003,16 +4994,16 @@
       <c r="J10" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
@@ -5020,10 +5011,10 @@
       <c r="V10" s="12"/>
     </row>
     <row r="11" spans="1:22">
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
@@ -5061,10 +5052,10 @@
       <c r="L12" s="14">
         <v>10</v>
       </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
@@ -5075,22 +5066,22 @@
       <c r="B13" s="14">
         <v>1</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>240</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>243</v>
       </c>
       <c r="I13" s="15" t="s">
@@ -5099,16 +5090,16 @@
       <c r="J13" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
@@ -5119,441 +5110,441 @@
       <c r="B14" s="14">
         <v>2</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>239</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="H14" s="18"/>
+      <c r="H14" s="16"/>
       <c r="I14" s="15" t="s">
         <v>241</v>
       </c>
       <c r="J14" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="L14" s="28"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="16" spans="1:22">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="21" t="s">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="19" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="22"/>
-      <c r="C17" s="26">
+      <c r="B17" s="20"/>
+      <c r="C17" s="24">
         <v>0</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="24">
         <v>1</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="24">
         <v>2</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="24">
         <v>3</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="24">
         <v>4</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="24">
         <v>5</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="24">
         <v>6</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="24">
         <v>7</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="24">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="24">
         <v>1</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="21">
         <v>1</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="21">
         <v>2</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="21">
         <v>3</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="21">
         <v>4</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="21">
         <v>5</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="21">
         <v>6</v>
       </c>
-      <c r="J18" s="23">
+      <c r="J18" s="21">
         <v>7</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="24">
         <v>2</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="21">
         <v>2</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="25">
         <v>2</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="21">
         <v>3</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="21">
         <v>4</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="21">
         <v>5</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="21">
         <v>6</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="21">
         <v>7</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="24">
         <v>3</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="21">
         <v>3</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="21">
         <v>3</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="22">
         <v>2</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="21">
         <v>3</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="21">
         <v>4</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="21">
         <v>5</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J20" s="21">
         <v>6</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="24">
         <v>4</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="21">
         <v>4</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="21">
         <v>4</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="21">
         <v>3</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="21">
         <v>3</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H21" s="21">
         <v>4</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="21">
         <v>5</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J21" s="21">
         <v>6</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="24">
         <v>5</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="21">
         <v>5</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="21">
         <v>5</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="21">
         <v>4</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="21">
         <v>4</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="21">
         <v>4</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="21">
         <v>5</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="21">
         <v>6</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="24">
         <v>6</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="21">
         <v>6</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="21">
         <v>6</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="21">
         <v>5</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="21">
         <v>5</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="25">
         <v>5</v>
       </c>
-      <c r="I23" s="23">
+      <c r="I23" s="21">
         <v>5</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="21">
         <v>6</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="24">
         <v>7</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="21">
         <v>7</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="21">
         <v>7</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <v>6</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="21">
         <v>6</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="21">
         <v>6</v>
       </c>
-      <c r="I24" s="24">
+      <c r="I24" s="22">
         <v>5</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="21">
         <v>6</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="24">
         <v>8</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="21">
         <v>8</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="21">
         <v>8</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="21">
         <v>7</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="21">
         <v>7</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="21">
         <v>7</v>
       </c>
-      <c r="I25" s="23">
+      <c r="I25" s="21">
         <v>6</v>
       </c>
-      <c r="J25" s="24">
+      <c r="J25" s="22">
         <v>5</v>
       </c>
-      <c r="K25" s="23">
+      <c r="K25" s="21">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="24">
         <v>9</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="21">
         <v>9</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="21">
         <v>9</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="21">
         <v>8</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="21">
         <v>8</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="21">
         <v>8</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="21">
         <v>7</v>
       </c>
-      <c r="J26" s="23">
+      <c r="J26" s="21">
         <v>6</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="21">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="24">
         <v>10</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="21">
         <v>10</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="21">
         <v>10</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="21">
         <v>9</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="21">
         <v>9</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H27" s="21">
         <v>9</v>
       </c>
-      <c r="I27" s="23">
+      <c r="I27" s="21">
         <v>8</v>
       </c>
-      <c r="J27" s="23">
+      <c r="J27" s="21">
         <v>7</v>
       </c>
-      <c r="K27" s="23">
+      <c r="K27" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="21" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="I30" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="J30" s="21" t="s">
+      <c r="J30" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="K30" s="21" t="s">
+      <c r="K30" s="19" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="22"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="14">
         <v>0</v>
       </c>
@@ -5583,322 +5574,322 @@
       </c>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="19" t="s">
         <v>238</v>
       </c>
       <c r="C32" s="14">
         <v>1</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="22">
         <v>1</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>2</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="21">
         <v>3</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="21">
         <v>4</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="21">
         <v>5</v>
       </c>
-      <c r="I32" s="23">
+      <c r="I32" s="21">
         <v>6</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="21">
         <v>7</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="2:11">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="19" t="s">
         <v>240</v>
       </c>
       <c r="C33" s="14">
         <v>2</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="21">
         <v>2</v>
       </c>
-      <c r="E33" s="24">
+      <c r="E33" s="22">
         <v>2</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="21">
         <v>3</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="21">
         <v>4</v>
       </c>
-      <c r="H33" s="23">
+      <c r="H33" s="21">
         <v>5</v>
       </c>
-      <c r="I33" s="23">
+      <c r="I33" s="21">
         <v>6</v>
       </c>
-      <c r="J33" s="23">
+      <c r="J33" s="21">
         <v>7</v>
       </c>
-      <c r="K33" s="23">
+      <c r="K33" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="2:11">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="19" t="s">
         <v>232</v>
       </c>
       <c r="C34" s="14">
         <v>3</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="21">
         <v>3</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>3</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="23">
         <v>2</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="21">
         <v>3</v>
       </c>
-      <c r="H34" s="23">
+      <c r="H34" s="21">
         <v>4</v>
       </c>
-      <c r="I34" s="23">
+      <c r="I34" s="21">
         <v>5</v>
       </c>
-      <c r="J34" s="23">
+      <c r="J34" s="21">
         <v>6</v>
       </c>
-      <c r="K34" s="23">
+      <c r="K34" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:11">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="19" t="s">
         <v>236</v>
       </c>
       <c r="C35" s="14">
         <v>4</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="21">
         <v>4</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>4</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="21">
         <v>3</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="22">
         <v>3</v>
       </c>
-      <c r="H35" s="23">
+      <c r="H35" s="21">
         <v>4</v>
       </c>
-      <c r="I35" s="23">
+      <c r="I35" s="21">
         <v>5</v>
       </c>
-      <c r="J35" s="23">
+      <c r="J35" s="21">
         <v>6</v>
       </c>
-      <c r="K35" s="23">
+      <c r="K35" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:11">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="19" t="s">
         <v>237</v>
       </c>
       <c r="C36" s="14">
         <v>5</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="21">
         <v>5</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="21">
         <v>5</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="21">
         <v>4</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="21">
         <v>4</v>
       </c>
-      <c r="H36" s="24">
+      <c r="H36" s="22">
         <v>4</v>
       </c>
-      <c r="I36" s="23">
+      <c r="I36" s="21">
         <v>5</v>
       </c>
-      <c r="J36" s="23">
+      <c r="J36" s="21">
         <v>6</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="2:11">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="19" t="s">
         <v>243</v>
       </c>
       <c r="C37" s="14">
         <v>6</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="21">
         <v>6</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="21">
         <v>6</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="21">
         <v>5</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="21">
         <v>5</v>
       </c>
-      <c r="H37" s="23">
+      <c r="H37" s="21">
         <v>5</v>
       </c>
-      <c r="I37" s="23">
+      <c r="I37" s="21">
         <v>5</v>
       </c>
-      <c r="J37" s="23">
+      <c r="J37" s="21">
         <v>6</v>
       </c>
-      <c r="K37" s="23">
+      <c r="K37" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="19" t="s">
         <v>241</v>
       </c>
       <c r="C38" s="14">
         <v>7</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="21">
         <v>7</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="21">
         <v>7</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="21">
         <v>6</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="21">
         <v>6</v>
       </c>
-      <c r="H38" s="23">
+      <c r="H38" s="21">
         <v>6</v>
       </c>
-      <c r="I38" s="25">
+      <c r="I38" s="23">
         <v>5</v>
       </c>
-      <c r="J38" s="23">
+      <c r="J38" s="21">
         <v>6</v>
       </c>
-      <c r="K38" s="23">
+      <c r="K38" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="19" t="s">
         <v>242</v>
       </c>
       <c r="C39" s="14">
         <v>8</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D39" s="21">
         <v>8</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="21">
         <v>8</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="21">
         <v>7</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="21">
         <v>7</v>
       </c>
-      <c r="H39" s="23">
+      <c r="H39" s="21">
         <v>7</v>
       </c>
-      <c r="I39" s="23">
+      <c r="I39" s="21">
         <v>6</v>
       </c>
-      <c r="J39" s="25">
+      <c r="J39" s="23">
         <v>5</v>
       </c>
-      <c r="K39" s="24">
+      <c r="K39" s="22">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="2:11">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="19" t="s">
         <v>243</v>
       </c>
       <c r="C40" s="14">
         <v>9</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="21">
         <v>9</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="21">
         <v>9</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="21">
         <v>8</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="21">
         <v>8</v>
       </c>
-      <c r="H40" s="23">
+      <c r="H40" s="21">
         <v>8</v>
       </c>
-      <c r="I40" s="23">
+      <c r="I40" s="21">
         <v>7</v>
       </c>
-      <c r="J40" s="23">
+      <c r="J40" s="21">
         <v>6</v>
       </c>
-      <c r="K40" s="23">
+      <c r="K40" s="21">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="2:11">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="19" t="s">
         <v>244</v>
       </c>
       <c r="C41" s="14">
         <v>10</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D41" s="21">
         <v>10</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="21">
         <v>10</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="21">
         <v>9</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="21">
         <v>9</v>
       </c>
-      <c r="H41" s="23">
+      <c r="H41" s="21">
         <v>9</v>
       </c>
-      <c r="I41" s="23">
+      <c r="I41" s="21">
         <v>8</v>
       </c>
-      <c r="J41" s="23">
+      <c r="J41" s="21">
         <v>7</v>
       </c>
-      <c r="K41" s="23">
+      <c r="K41" s="21">
         <v>7</v>
       </c>
     </row>

</xml_diff>